<commit_message>
fix 契約管理_随時対応_値上げ更新 Signed-off-by: LiuYiyang <lyy@shequchina.cn>
</commit_message>
<xml_diff>
--- a/test_物件管理/已完成/test_契約管理_随時対応_値上げ更新_new.xlsx
+++ b/test_物件管理/已完成/test_契約管理_随時対応_値上げ更新_new.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" tabRatio="758" firstSheet="6" activeTab="11"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" tabRatio="758" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="IN_DB_001" sheetId="7" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8224" uniqueCount="1025">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8227" uniqueCount="1028">
   <si>
     <t>URL:</t>
   </si>
@@ -2536,9 +2536,6 @@
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
   <si>
-    <t>/html/body/main/div/div[1]/div/div/div/table/tbody/tr[2]/td[2]/a</t>
-  </si>
-  <si>
     <t>テスト2</t>
   </si>
   <si>
@@ -3385,6 +3382,18 @@
     <t>97979</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
+  <si>
+    <t>HOME</t>
+  </si>
+  <si>
+    <t>/html/body/main/div/div[1]/div/div/div/table/thead/tr/th[1]</t>
+  </si>
+  <si>
+    <t>排序</t>
+  </si>
+  <si>
+    <t>/html/body/main/div/div[1]/div/div/div/table/tbody/tr[3]/td[2]/a</t>
+  </si>
 </sst>
 </file>
 
@@ -3397,7 +3406,7 @@
     <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="36">
+  <fonts count="37">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3646,6 +3655,14 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -3739,7 +3756,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="65">
+  <cellStyleXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
@@ -3843,8 +3860,9 @@
     <xf numFmtId="43" fontId="23" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="33" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="33" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="203">
+  <cellXfs count="205">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4304,8 +4322,12 @@
     <xf numFmtId="49" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="65">
+  <cellStyles count="66">
     <cellStyle name="Comma [0]" xfId="38"/>
     <cellStyle name="Comma [0] 2" xfId="43"/>
     <cellStyle name="Comma [0] 3" xfId="54"/>
@@ -4344,6 +4366,7 @@
     <cellStyle name="常规 2 2" xfId="23"/>
     <cellStyle name="常规 2 3" xfId="21"/>
     <cellStyle name="常规 2 4" xfId="36"/>
+    <cellStyle name="常规 2 5" xfId="65"/>
     <cellStyle name="常规 3" xfId="3"/>
     <cellStyle name="常规 3 2" xfId="13"/>
     <cellStyle name="常规 3 3" xfId="45"/>
@@ -13742,7 +13765,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="171" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="171" customFormat="1" ht="14.25">
@@ -13756,10 +13779,10 @@
         <v>18</v>
       </c>
       <c r="B4" s="171" t="s">
+        <v>794</v>
+      </c>
+      <c r="I4" s="171" t="s">
         <v>795</v>
-      </c>
-      <c r="I4" s="171" t="s">
-        <v>796</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="122" customFormat="1" ht="14.25">
@@ -13781,19 +13804,19 @@
     </row>
     <row r="7" spans="1:9" s="171" customFormat="1" ht="14.25">
       <c r="A7" s="180" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="B7" s="151" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="C7" s="173"/>
     </row>
     <row r="8" spans="1:9" s="171" customFormat="1" ht="14.25">
       <c r="A8" s="180" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="B8" s="187" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="C8" s="173"/>
     </row>
@@ -13802,21 +13825,21 @@
         <v>4</v>
       </c>
       <c r="B9" s="183" t="s">
+        <v>973</v>
+      </c>
+      <c r="C9" s="184" t="s">
+        <v>977</v>
+      </c>
+      <c r="D9" s="182" t="s">
         <v>974</v>
-      </c>
-      <c r="C9" s="184" t="s">
-        <v>978</v>
-      </c>
-      <c r="D9" s="182" t="s">
-        <v>975</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="171" customFormat="1" ht="14.25">
       <c r="A10" s="180" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="B10" s="171" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="171" customFormat="1" ht="14.25">
@@ -13824,21 +13847,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="183" t="s">
+        <v>973</v>
+      </c>
+      <c r="C11" s="184" t="s">
+        <v>979</v>
+      </c>
+      <c r="D11" s="182" t="s">
         <v>974</v>
-      </c>
-      <c r="C11" s="184" t="s">
-        <v>980</v>
-      </c>
-      <c r="D11" s="182" t="s">
-        <v>975</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="171" customFormat="1" ht="14.25">
       <c r="A12" s="180" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="B12" s="171" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="171" customFormat="1" ht="14.25">
@@ -13849,10 +13872,10 @@
         <v>600</v>
       </c>
       <c r="C13" s="184" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="D13" s="182" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="171" customFormat="1" ht="14.25">
@@ -13872,10 +13895,10 @@
         <v>18</v>
       </c>
       <c r="B16" s="171" t="s">
+        <v>985</v>
+      </c>
+      <c r="H16" s="171" t="s">
         <v>986</v>
-      </c>
-      <c r="H16" s="171" t="s">
-        <v>987</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="14.25">
@@ -13912,10 +13935,10 @@
     </row>
     <row r="22" spans="1:8" ht="14.25">
       <c r="A22" s="180" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="B22" s="171" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
   </sheetData>
@@ -14109,7 +14132,7 @@
         <v>735</v>
       </c>
       <c r="J4" s="185" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="K4" s="186" t="s">
         <v>170</v>
@@ -16675,25 +16698,25 @@
         <v>228</v>
       </c>
       <c r="H22" s="185" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="I22" s="185" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="J22" s="185" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="K22" s="185" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="L22" s="185" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="M22" s="185" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="N22" s="185" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="O22" s="185" t="s">
         <v>684</v>
@@ -16705,7 +16728,7 @@
         <v>229</v>
       </c>
       <c r="R22" s="185" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="S22" s="186" t="s">
         <v>170</v>
@@ -16732,22 +16755,22 @@
         <v>170</v>
       </c>
       <c r="AA22" s="185" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="AB22" s="185" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="AC22" s="185" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="AD22" s="185" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="AE22" s="185" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="AF22" s="185" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="AG22" s="186" t="s">
         <v>170</v>
@@ -16771,31 +16794,31 @@
         <v>170</v>
       </c>
       <c r="AN22" s="185" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="AO22" s="185" t="s">
         <v>228</v>
       </c>
       <c r="AP22" s="185" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="AQ22" s="185" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="AR22" s="185" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="AS22" s="185" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="AT22" s="185" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="AU22" s="185" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="AV22" s="185" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="AW22" s="186" t="s">
         <v>170</v>
@@ -16846,31 +16869,31 @@
         <v>170</v>
       </c>
       <c r="BM22" s="185" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="BN22" s="185" t="s">
+        <v>945</v>
+      </c>
+      <c r="BO22" s="186" t="s">
+        <v>170</v>
+      </c>
+      <c r="BP22" s="186" t="s">
+        <v>170</v>
+      </c>
+      <c r="BQ22" s="186" t="s">
+        <v>170</v>
+      </c>
+      <c r="BR22" s="186" t="s">
+        <v>170</v>
+      </c>
+      <c r="BS22" s="186" t="s">
+        <v>170</v>
+      </c>
+      <c r="BT22" s="185" t="s">
         <v>946</v>
       </c>
-      <c r="BO22" s="186" t="s">
-        <v>170</v>
-      </c>
-      <c r="BP22" s="186" t="s">
-        <v>170</v>
-      </c>
-      <c r="BQ22" s="186" t="s">
-        <v>170</v>
-      </c>
-      <c r="BR22" s="186" t="s">
-        <v>170</v>
-      </c>
-      <c r="BS22" s="186" t="s">
-        <v>170</v>
-      </c>
-      <c r="BT22" s="185" t="s">
-        <v>947</v>
-      </c>
       <c r="BU22" s="185" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="BV22" s="186" t="s">
         <v>170</v>
@@ -16879,7 +16902,7 @@
         <v>170</v>
       </c>
       <c r="BX22" s="185" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="BY22" s="186" t="s">
         <v>170</v>
@@ -16891,19 +16914,19 @@
         <v>170</v>
       </c>
       <c r="CB22" s="185" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="CC22" s="185" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="CD22" s="185" t="s">
         <v>615</v>
       </c>
       <c r="CE22" s="185" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="CF22" s="185" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="CG22" s="186" t="s">
         <v>170</v>
@@ -16912,16 +16935,16 @@
         <v>170</v>
       </c>
       <c r="CI22" s="185" t="s">
+        <v>948</v>
+      </c>
+      <c r="CJ22" s="185" t="s">
         <v>949</v>
       </c>
-      <c r="CJ22" s="185" t="s">
+      <c r="CK22" s="185" t="s">
         <v>950</v>
       </c>
-      <c r="CK22" s="185" t="s">
-        <v>951</v>
-      </c>
       <c r="CL22" s="185" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="CM22" s="186" t="s">
         <v>170</v>
@@ -16939,22 +16962,22 @@
         <v>220</v>
       </c>
       <c r="CR22" s="185" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="CS22" s="186" t="s">
         <v>170</v>
       </c>
       <c r="CT22" s="185" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="CU22" s="185" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="CV22" s="186" t="s">
         <v>170</v>
       </c>
       <c r="CW22" s="185" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="CX22" s="186" t="s">
         <v>170</v>
@@ -17002,13 +17025,13 @@
         <v>170</v>
       </c>
       <c r="DM22" s="185" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="DN22" s="185" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="DO22" s="185" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="DP22" s="186" t="s">
         <v>170</v>
@@ -19012,17 +19035,17 @@
         <v>250</v>
       </c>
       <c r="B35" s="175" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="36" spans="1:142" s="171" customFormat="1">
       <c r="B36" s="179" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="37" spans="1:142" s="171" customFormat="1">
       <c r="B37" s="178" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="C37" s="177" t="s">
         <v>19</v>
@@ -19037,10 +19060,10 @@
         <v>21</v>
       </c>
       <c r="G37" s="177" t="s">
+        <v>994</v>
+      </c>
+      <c r="H37" s="177" t="s">
         <v>995</v>
-      </c>
-      <c r="H37" s="177" t="s">
-        <v>996</v>
       </c>
       <c r="I37" s="177" t="s">
         <v>43</v>
@@ -19049,28 +19072,28 @@
         <v>37</v>
       </c>
       <c r="K37" s="177" t="s">
+        <v>996</v>
+      </c>
+      <c r="L37" s="177" t="s">
         <v>997</v>
       </c>
-      <c r="L37" s="177" t="s">
+      <c r="M37" s="177" t="s">
         <v>998</v>
       </c>
-      <c r="M37" s="177" t="s">
+      <c r="N37" s="177" t="s">
         <v>999</v>
       </c>
-      <c r="N37" s="177" t="s">
+      <c r="O37" s="177" t="s">
         <v>1000</v>
       </c>
-      <c r="O37" s="177" t="s">
+      <c r="P37" s="177" t="s">
         <v>1001</v>
       </c>
-      <c r="P37" s="177" t="s">
+      <c r="Q37" s="177" t="s">
         <v>1002</v>
       </c>
-      <c r="Q37" s="177" t="s">
+      <c r="R37" s="177" t="s">
         <v>1003</v>
-      </c>
-      <c r="R37" s="177" t="s">
-        <v>1004</v>
       </c>
       <c r="S37" s="177" t="s">
         <v>440</v>
@@ -19088,25 +19111,25 @@
         <v>36</v>
       </c>
       <c r="X37" s="177" t="s">
+        <v>1004</v>
+      </c>
+      <c r="Y37" s="177" t="s">
         <v>1005</v>
       </c>
-      <c r="Y37" s="177" t="s">
+      <c r="Z37" s="177" t="s">
         <v>1006</v>
       </c>
-      <c r="Z37" s="177" t="s">
+      <c r="AA37" s="177" t="s">
         <v>1007</v>
       </c>
-      <c r="AA37" s="177" t="s">
+      <c r="AB37" s="177" t="s">
         <v>1008</v>
       </c>
-      <c r="AB37" s="177" t="s">
+      <c r="AC37" s="177" t="s">
         <v>1009</v>
       </c>
-      <c r="AC37" s="177" t="s">
+      <c r="AD37" s="177" t="s">
         <v>1010</v>
-      </c>
-      <c r="AD37" s="177" t="s">
-        <v>1011</v>
       </c>
     </row>
     <row r="38" spans="1:142" s="171" customFormat="1">
@@ -19177,16 +19200,16 @@
         <v>2</v>
       </c>
       <c r="X38" s="201" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="Y38" s="185">
         <v>105817</v>
       </c>
       <c r="Z38" s="185" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="AA38" s="185" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="AB38" s="185">
         <v>1</v>
@@ -19214,7 +19237,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:BP69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
@@ -19283,7 +19306,7 @@
     </row>
     <row r="5" spans="2:68" s="139" customFormat="1" ht="12">
       <c r="B5" s="139" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="C5" s="139" t="s">
         <v>686</v>
@@ -19295,12 +19318,12 @@
         <v>713</v>
       </c>
       <c r="F5" s="151" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="6" spans="2:68" s="139" customFormat="1" ht="12">
       <c r="B6" s="139" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="7" spans="2:68" s="139" customFormat="1" ht="12">
@@ -19321,10 +19344,10 @@
         <v>715</v>
       </c>
       <c r="E9" s="139" t="s">
+        <v>787</v>
+      </c>
+      <c r="F9" s="139" t="s">
         <v>788</v>
-      </c>
-      <c r="F9" s="139" t="s">
-        <v>789</v>
       </c>
       <c r="J9" s="151"/>
     </row>
@@ -19349,7 +19372,7 @@
     </row>
     <row r="12" spans="2:68" s="139" customFormat="1" ht="12">
       <c r="B12" s="151" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="L12" s="151"/>
     </row>
@@ -19361,7 +19384,7 @@
     </row>
     <row r="14" spans="2:68" s="139" customFormat="1" ht="12">
       <c r="B14" s="151" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="D14" s="151" t="s">
         <v>717</v>
@@ -19400,18 +19423,18 @@
         <v>773</v>
       </c>
       <c r="D19" s="151" t="s">
+        <v>970</v>
+      </c>
+      <c r="E19" s="151" t="s">
         <v>971</v>
       </c>
-      <c r="E19" s="151" t="s">
+      <c r="F19" s="151" t="s">
         <v>972</v>
-      </c>
-      <c r="F19" s="151" t="s">
-        <v>973</v>
       </c>
     </row>
     <row r="20" spans="1:68" s="139" customFormat="1" ht="12">
       <c r="B20" s="151" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="21" spans="1:68" s="139" customFormat="1" ht="12">
@@ -19427,7 +19450,7 @@
     </row>
     <row r="23" spans="1:68" s="139" customFormat="1" ht="12">
       <c r="B23" s="151" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="L23" s="151"/>
     </row>
@@ -19675,10 +19698,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -19693,206 +19716,240 @@
     </row>
     <row r="2" spans="1:10" s="138" customFormat="1"/>
     <row r="3" spans="1:10" s="138" customFormat="1" ht="14.25">
-      <c r="A3" s="134" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" s="138" customFormat="1" ht="14.25">
-      <c r="A4" s="134" t="s">
+      <c r="A3" s="204" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B3" s="203"/>
+      <c r="C3" s="203"/>
+      <c r="D3" s="203"/>
+      <c r="E3" s="203"/>
+      <c r="F3" s="203"/>
+      <c r="G3" s="203"/>
+      <c r="H3" s="203"/>
+      <c r="I3" s="203"/>
+      <c r="J3" s="203"/>
+    </row>
+    <row r="4" spans="1:10" s="192" customFormat="1" ht="14.25">
+      <c r="A4" s="204" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="138" t="s">
+      <c r="B4" s="203" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C4" s="203"/>
+      <c r="D4" s="203"/>
+      <c r="E4" s="203"/>
+      <c r="F4" s="203"/>
+      <c r="G4" s="203"/>
+      <c r="H4" s="203"/>
+      <c r="I4" s="203" t="s">
+        <v>1026</v>
+      </c>
+      <c r="J4" s="203"/>
+    </row>
+    <row r="5" spans="1:10" s="138" customFormat="1" ht="14.25">
+      <c r="A5" s="204" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="203" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C5" s="203"/>
+      <c r="D5" s="203"/>
+      <c r="E5" s="203"/>
+      <c r="F5" s="203"/>
+      <c r="G5" s="203"/>
+      <c r="H5" s="203"/>
+      <c r="I5" s="203" t="s">
         <v>778</v>
       </c>
-      <c r="I4" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="14.25">
-      <c r="A5" s="134" t="s">
-        <v>780</v>
-      </c>
-      <c r="B5" s="99"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
+      <c r="J5" s="203"/>
     </row>
     <row r="6" spans="1:10" ht="14.25">
       <c r="A6" s="134" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="64" t="s">
-        <v>781</v>
-      </c>
+        <v>779</v>
+      </c>
+      <c r="B6" s="99"/>
       <c r="C6" s="41"/>
       <c r="D6" s="64"/>
       <c r="E6" s="64"/>
       <c r="F6" s="64"/>
-      <c r="I6" s="138" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="42" customFormat="1" ht="14.25">
-      <c r="A7" s="77" t="s">
+    </row>
+    <row r="7" spans="1:10" ht="14.25">
+      <c r="A7" s="134" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="64" t="s">
-        <v>591</v>
+        <v>780</v>
       </c>
       <c r="C7" s="41"/>
       <c r="D7" s="64"/>
       <c r="E7" s="64"/>
       <c r="F7" s="64"/>
       <c r="I7" s="138" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="64" customFormat="1" ht="14.25">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="42" customFormat="1" ht="14.25">
       <c r="A8" s="77" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="64" t="s">
+        <v>591</v>
+      </c>
+      <c r="C8" s="41"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="I8" s="138" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="64" customFormat="1" ht="14.25">
+      <c r="A9" s="77" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="64" t="s">
         <v>687</v>
       </c>
-      <c r="C8" s="52"/>
-      <c r="I8" s="138" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="14.25">
-      <c r="A9" s="77" t="s">
-        <v>688</v>
-      </c>
-      <c r="B9" s="111" t="s">
-        <v>787</v>
+      <c r="C9" s="52"/>
+      <c r="I9" s="138" t="s">
+        <v>783</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="14.25">
       <c r="A10" s="77" t="s">
+        <v>688</v>
+      </c>
+      <c r="B10" s="111" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="14.25">
+      <c r="A11" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B11" s="42" t="s">
         <v>592</v>
       </c>
-      <c r="I10" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="14.25">
-      <c r="A11" s="134" t="s">
-        <v>780</v>
-      </c>
-      <c r="B11" s="109"/>
+      <c r="I11" t="s">
+        <v>784</v>
+      </c>
     </row>
     <row r="12" spans="1:10" ht="14.25">
       <c r="A12" s="134" t="s">
+        <v>779</v>
+      </c>
+      <c r="B12" s="109"/>
+    </row>
+    <row r="13" spans="1:10" ht="14.25">
+      <c r="A13" s="134" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="67" t="s">
+      <c r="B13" s="67" t="s">
+        <v>789</v>
+      </c>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="I13" t="s">
         <v>790</v>
       </c>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="I12" t="s">
-        <v>791</v>
-      </c>
-      <c r="J12" s="42"/>
-    </row>
-    <row r="13" spans="1:10" s="138" customFormat="1" ht="14.25">
-      <c r="A13" s="134" t="s">
-        <v>517</v>
-      </c>
-      <c r="B13" s="138" t="s">
-        <v>798</v>
-      </c>
+      <c r="J13" s="42"/>
     </row>
     <row r="14" spans="1:10" s="138" customFormat="1" ht="14.25">
       <c r="A14" s="134" t="s">
+        <v>517</v>
+      </c>
+      <c r="B14" s="138" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="138" customFormat="1" ht="14.25">
+      <c r="A15" s="134" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="138" t="s">
-        <v>794</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="171" customFormat="1" ht="14.25">
-      <c r="A15" s="180" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="138" customFormat="1" ht="14.25">
-      <c r="A16" s="134" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="138" t="s">
-        <v>795</v>
-      </c>
-      <c r="I16" s="138" t="s">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="14.25">
+      <c r="B15" s="138" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="171" customFormat="1" ht="14.25">
+      <c r="A16" s="180" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="138" customFormat="1" ht="14.25">
       <c r="A17" s="134" t="s">
         <v>18</v>
       </c>
-      <c r="B17" t="s">
-        <v>792</v>
+      <c r="B17" s="138" t="s">
+        <v>794</v>
       </c>
       <c r="I17" s="138" t="s">
-        <v>799</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" s="138" customFormat="1" ht="14.25">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="14.25">
       <c r="A18" s="134" t="s">
-        <v>517</v>
-      </c>
-      <c r="B18" s="138" t="s">
-        <v>800</v>
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>791</v>
+      </c>
+      <c r="I18" s="138" t="s">
+        <v>798</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="138" customFormat="1" ht="14.25">
       <c r="A19" s="134" t="s">
+        <v>517</v>
+      </c>
+      <c r="B19" s="138" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="138" customFormat="1" ht="14.25">
+      <c r="A20" s="134" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="138" t="s">
-        <v>794</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" s="171" customFormat="1" ht="14.25">
-      <c r="A20" s="180" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" s="138" customFormat="1" ht="14.25">
-      <c r="A21" s="134" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="138" t="s">
-        <v>795</v>
-      </c>
-      <c r="I21" s="138" t="s">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="14.25">
+      <c r="B20" s="138" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="171" customFormat="1" ht="14.25">
+      <c r="A21" s="180" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="138" customFormat="1" ht="14.25">
       <c r="A22" s="134" t="s">
         <v>18</v>
       </c>
-      <c r="B22" t="s">
-        <v>793</v>
+      <c r="B22" s="138" t="s">
+        <v>794</v>
       </c>
       <c r="I22" s="138" t="s">
-        <v>801</v>
+        <v>795</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="14.25">
       <c r="A23" s="134" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" t="s">
+        <v>792</v>
+      </c>
+      <c r="I23" s="138" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="14.25">
+      <c r="A24" s="134" t="s">
         <v>517</v>
       </c>
-      <c r="B23" s="138" t="s">
-        <v>802</v>
+      <c r="B24" s="138" t="s">
+        <v>801</v>
       </c>
     </row>
   </sheetData>
@@ -22652,7 +22709,7 @@
         <v>228</v>
       </c>
       <c r="H22" s="163" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="I22" s="164" t="s">
         <v>170</v>
@@ -22892,13 +22949,13 @@
         <v>170</v>
       </c>
       <c r="CJ22" s="163" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="CK22" s="163" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="CL22" s="163" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="CM22" s="164" t="s">
         <v>170</v>
@@ -24793,17 +24850,17 @@
         <v>250</v>
       </c>
       <c r="B34" s="175" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="35" spans="1:30" s="171" customFormat="1">
       <c r="B35" s="179" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="36" spans="1:30" s="171" customFormat="1">
       <c r="B36" s="178" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="C36" s="177" t="s">
         <v>19</v>
@@ -24818,10 +24875,10 @@
         <v>21</v>
       </c>
       <c r="G36" s="177" t="s">
+        <v>994</v>
+      </c>
+      <c r="H36" s="177" t="s">
         <v>995</v>
-      </c>
-      <c r="H36" s="177" t="s">
-        <v>996</v>
       </c>
       <c r="I36" s="177" t="s">
         <v>43</v>
@@ -24830,28 +24887,28 @@
         <v>37</v>
       </c>
       <c r="K36" s="177" t="s">
+        <v>996</v>
+      </c>
+      <c r="L36" s="177" t="s">
         <v>997</v>
       </c>
-      <c r="L36" s="177" t="s">
+      <c r="M36" s="177" t="s">
         <v>998</v>
       </c>
-      <c r="M36" s="177" t="s">
+      <c r="N36" s="177" t="s">
         <v>999</v>
       </c>
-      <c r="N36" s="177" t="s">
+      <c r="O36" s="177" t="s">
         <v>1000</v>
       </c>
-      <c r="O36" s="177" t="s">
+      <c r="P36" s="177" t="s">
         <v>1001</v>
       </c>
-      <c r="P36" s="177" t="s">
+      <c r="Q36" s="177" t="s">
         <v>1002</v>
       </c>
-      <c r="Q36" s="177" t="s">
+      <c r="R36" s="177" t="s">
         <v>1003</v>
-      </c>
-      <c r="R36" s="177" t="s">
-        <v>1004</v>
       </c>
       <c r="S36" s="177" t="s">
         <v>440</v>
@@ -24869,25 +24926,25 @@
         <v>36</v>
       </c>
       <c r="X36" s="177" t="s">
+        <v>1004</v>
+      </c>
+      <c r="Y36" s="177" t="s">
         <v>1005</v>
       </c>
-      <c r="Y36" s="177" t="s">
+      <c r="Z36" s="177" t="s">
         <v>1006</v>
       </c>
-      <c r="Z36" s="177" t="s">
+      <c r="AA36" s="177" t="s">
         <v>1007</v>
       </c>
-      <c r="AA36" s="177" t="s">
+      <c r="AB36" s="177" t="s">
         <v>1008</v>
       </c>
-      <c r="AB36" s="177" t="s">
+      <c r="AC36" s="177" t="s">
         <v>1009</v>
       </c>
-      <c r="AC36" s="177" t="s">
+      <c r="AD36" s="177" t="s">
         <v>1010</v>
-      </c>
-      <c r="AD36" s="177" t="s">
-        <v>1011</v>
       </c>
     </row>
     <row r="37" spans="1:30" s="171" customFormat="1">
@@ -24910,13 +24967,13 @@
         <v>2019</v>
       </c>
       <c r="H37" s="185" t="s">
+        <v>1017</v>
+      </c>
+      <c r="I37" s="185" t="s">
+        <v>1014</v>
+      </c>
+      <c r="J37" s="185" t="s">
         <v>1018</v>
-      </c>
-      <c r="I37" s="185" t="s">
-        <v>1015</v>
-      </c>
-      <c r="J37" s="185" t="s">
-        <v>1019</v>
       </c>
       <c r="K37" s="185">
         <v>20000</v>
@@ -25011,7 +25068,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="138" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
@@ -25025,10 +25082,10 @@
         <v>18</v>
       </c>
       <c r="B4" s="138" t="s">
+        <v>794</v>
+      </c>
+      <c r="I4" s="138" t="s">
         <v>795</v>
-      </c>
-      <c r="I4" s="138" t="s">
-        <v>796</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="14.25">
@@ -25036,15 +25093,15 @@
         <v>18</v>
       </c>
       <c r="B5" s="138" t="s">
+        <v>802</v>
+      </c>
+      <c r="I5" s="138" t="s">
         <v>803</v>
-      </c>
-      <c r="I5" s="138" t="s">
-        <v>804</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="140" customFormat="1" ht="14.25">
       <c r="A6" s="150" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="140" customFormat="1" ht="14.25">
@@ -25052,17 +25109,17 @@
         <v>0</v>
       </c>
       <c r="B7" s="140" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="140" customFormat="1" ht="14.25">
       <c r="A8" s="150" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="14.25">
       <c r="A9" s="150" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="14.25">
@@ -25070,13 +25127,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="156" t="s">
+        <v>804</v>
+      </c>
+      <c r="C10" s="157" t="s">
         <v>805</v>
       </c>
-      <c r="C10" s="157" t="s">
+      <c r="D10" s="155" t="s">
         <v>806</v>
-      </c>
-      <c r="D10" s="155" t="s">
-        <v>807</v>
       </c>
       <c r="E10" s="140"/>
       <c r="F10" s="140"/>
@@ -25087,13 +25144,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="156" t="s">
+        <v>941</v>
+      </c>
+      <c r="C11" s="157" t="s">
+        <v>940</v>
+      </c>
+      <c r="D11" s="153" t="s">
         <v>942</v>
-      </c>
-      <c r="C11" s="157" t="s">
-        <v>941</v>
-      </c>
-      <c r="D11" s="153" t="s">
-        <v>943</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="14.25">
@@ -25101,13 +25158,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="156" t="s">
+        <v>807</v>
+      </c>
+      <c r="C12" s="184" t="s">
+        <v>962</v>
+      </c>
+      <c r="D12" s="155" t="s">
         <v>808</v>
-      </c>
-      <c r="C12" s="184" t="s">
-        <v>963</v>
-      </c>
-      <c r="D12" s="155" t="s">
-        <v>809</v>
       </c>
       <c r="E12" s="140"/>
       <c r="F12" s="140"/>
@@ -25118,13 +25175,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="156" t="s">
+        <v>809</v>
+      </c>
+      <c r="C13" s="157" t="s">
         <v>810</v>
       </c>
-      <c r="C13" s="157" t="s">
+      <c r="D13" s="155" t="s">
         <v>811</v>
-      </c>
-      <c r="D13" s="155" t="s">
-        <v>812</v>
       </c>
       <c r="E13" s="140"/>
       <c r="F13" s="140"/>
@@ -25135,13 +25192,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="156" t="s">
+        <v>915</v>
+      </c>
+      <c r="C14" s="157" t="s">
         <v>916</v>
       </c>
-      <c r="C14" s="157" t="s">
+      <c r="D14" s="155" t="s">
         <v>917</v>
-      </c>
-      <c r="D14" s="155" t="s">
-        <v>918</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="14.25">
@@ -25149,13 +25206,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="156" t="s">
+        <v>812</v>
+      </c>
+      <c r="C15" s="157" t="s">
+        <v>918</v>
+      </c>
+      <c r="D15" s="155" t="s">
         <v>813</v>
-      </c>
-      <c r="C15" s="157" t="s">
-        <v>919</v>
-      </c>
-      <c r="D15" s="155" t="s">
-        <v>814</v>
       </c>
       <c r="E15" s="140"/>
       <c r="F15" s="140"/>
@@ -25166,13 +25223,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="156" t="s">
+        <v>814</v>
+      </c>
+      <c r="C16" s="157" t="s">
+        <v>919</v>
+      </c>
+      <c r="D16" s="155" t="s">
         <v>815</v>
-      </c>
-      <c r="C16" s="157" t="s">
-        <v>920</v>
-      </c>
-      <c r="D16" s="155" t="s">
-        <v>816</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25">
@@ -25180,13 +25237,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="156" t="s">
+        <v>816</v>
+      </c>
+      <c r="C17" s="157" t="s">
         <v>817</v>
       </c>
-      <c r="C17" s="157" t="s">
+      <c r="D17" s="155" t="s">
         <v>818</v>
-      </c>
-      <c r="D17" s="155" t="s">
-        <v>819</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.25">
@@ -25194,13 +25251,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="156" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="C18" s="157">
         <v>13911110000</v>
       </c>
       <c r="D18" s="155" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25">
@@ -25208,13 +25265,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="156" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="C19" s="157" t="s">
         <v>684</v>
       </c>
       <c r="D19" s="155" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.25">
@@ -25222,13 +25279,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="156" t="s">
+        <v>823</v>
+      </c>
+      <c r="C20" s="157" t="s">
         <v>824</v>
       </c>
-      <c r="C20" s="157" t="s">
+      <c r="D20" s="155" t="s">
         <v>825</v>
-      </c>
-      <c r="D20" s="155" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.25">
@@ -25236,13 +25293,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="156" t="s">
+        <v>826</v>
+      </c>
+      <c r="C21" s="157" t="s">
         <v>827</v>
       </c>
-      <c r="C21" s="157" t="s">
+      <c r="D21" s="155" t="s">
         <v>828</v>
-      </c>
-      <c r="D21" s="155" t="s">
-        <v>829</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="14.25">
@@ -25250,13 +25307,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="156" t="s">
+        <v>829</v>
+      </c>
+      <c r="C22" s="157" t="s">
         <v>830</v>
       </c>
-      <c r="C22" s="157" t="s">
+      <c r="D22" s="155" t="s">
         <v>831</v>
-      </c>
-      <c r="D22" s="155" t="s">
-        <v>832</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.25">
@@ -25264,13 +25321,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="156" t="s">
+        <v>832</v>
+      </c>
+      <c r="C23" s="157" t="s">
         <v>833</v>
       </c>
-      <c r="C23" s="157" t="s">
+      <c r="D23" s="155" t="s">
         <v>834</v>
-      </c>
-      <c r="D23" s="155" t="s">
-        <v>835</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14.25">
@@ -25278,13 +25335,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="156" t="s">
+        <v>835</v>
+      </c>
+      <c r="C24" s="157" t="s">
         <v>836</v>
       </c>
-      <c r="C24" s="157" t="s">
+      <c r="D24" s="155" t="s">
         <v>837</v>
-      </c>
-      <c r="D24" s="155" t="s">
-        <v>838</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.25">
@@ -25292,13 +25349,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="156" t="s">
+        <v>838</v>
+      </c>
+      <c r="C25" s="157" t="s">
         <v>839</v>
       </c>
-      <c r="C25" s="157" t="s">
+      <c r="D25" s="155" t="s">
         <v>840</v>
-      </c>
-      <c r="D25" s="155" t="s">
-        <v>841</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="14.25">
@@ -25306,7 +25363,7 @@
       <c r="B26" s="156"/>
       <c r="C26" s="157"/>
       <c r="D26" s="154" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.25">
@@ -25314,10 +25371,10 @@
         <v>4</v>
       </c>
       <c r="B27" s="156" t="s">
+        <v>842</v>
+      </c>
+      <c r="C27" s="157" t="s">
         <v>843</v>
-      </c>
-      <c r="C27" s="157" t="s">
-        <v>844</v>
       </c>
       <c r="D27" s="155" t="s">
         <v>613</v>
@@ -25328,13 +25385,13 @@
         <v>4</v>
       </c>
       <c r="B28" s="156" t="s">
+        <v>921</v>
+      </c>
+      <c r="C28" s="157" t="s">
+        <v>920</v>
+      </c>
+      <c r="D28" s="155" t="s">
         <v>922</v>
-      </c>
-      <c r="C28" s="157" t="s">
-        <v>921</v>
-      </c>
-      <c r="D28" s="155" t="s">
-        <v>923</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.25">
@@ -25342,13 +25399,13 @@
         <v>4</v>
       </c>
       <c r="B29" s="156" t="s">
+        <v>844</v>
+      </c>
+      <c r="C29" s="184" t="s">
+        <v>963</v>
+      </c>
+      <c r="D29" s="155" t="s">
         <v>845</v>
-      </c>
-      <c r="C29" s="184" t="s">
-        <v>964</v>
-      </c>
-      <c r="D29" s="155" t="s">
-        <v>846</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.25">
@@ -25356,13 +25413,13 @@
         <v>4</v>
       </c>
       <c r="B30" s="156" t="s">
+        <v>846</v>
+      </c>
+      <c r="C30" s="157" t="s">
+        <v>924</v>
+      </c>
+      <c r="D30" s="155" t="s">
         <v>847</v>
-      </c>
-      <c r="C30" s="157" t="s">
-        <v>925</v>
-      </c>
-      <c r="D30" s="155" t="s">
-        <v>848</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14.25">
@@ -25370,13 +25427,13 @@
         <v>4</v>
       </c>
       <c r="B31" s="156" t="s">
+        <v>848</v>
+      </c>
+      <c r="C31" s="157" t="s">
         <v>849</v>
       </c>
-      <c r="C31" s="157" t="s">
+      <c r="D31" s="155" t="s">
         <v>850</v>
-      </c>
-      <c r="D31" s="155" t="s">
-        <v>851</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="14.25">
@@ -25384,13 +25441,13 @@
         <v>4</v>
       </c>
       <c r="B32" s="156" t="s">
+        <v>851</v>
+      </c>
+      <c r="C32" s="157" t="s">
         <v>852</v>
       </c>
-      <c r="C32" s="157" t="s">
+      <c r="D32" s="155" t="s">
         <v>853</v>
-      </c>
-      <c r="D32" s="155" t="s">
-        <v>854</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.25">
@@ -25398,13 +25455,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="156" t="s">
+        <v>854</v>
+      </c>
+      <c r="C33" s="157" t="s">
         <v>855</v>
       </c>
-      <c r="C33" s="157" t="s">
+      <c r="D33" s="155" t="s">
         <v>856</v>
-      </c>
-      <c r="D33" s="155" t="s">
-        <v>857</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="14.25">
@@ -25412,13 +25469,13 @@
         <v>4</v>
       </c>
       <c r="B34" s="156" t="s">
+        <v>857</v>
+      </c>
+      <c r="C34" s="157" t="s">
         <v>858</v>
       </c>
-      <c r="C34" s="157" t="s">
+      <c r="D34" s="155" t="s">
         <v>859</v>
-      </c>
-      <c r="D34" s="155" t="s">
-        <v>860</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="14.25">
@@ -25426,10 +25483,10 @@
         <v>4</v>
       </c>
       <c r="B35" s="156" t="s">
+        <v>860</v>
+      </c>
+      <c r="C35" s="157" t="s">
         <v>861</v>
-      </c>
-      <c r="C35" s="157" t="s">
-        <v>862</v>
       </c>
       <c r="D35" s="155" t="s">
         <v>614</v>
@@ -25440,13 +25497,13 @@
         <v>4</v>
       </c>
       <c r="B36" s="156" t="s">
+        <v>862</v>
+      </c>
+      <c r="C36" s="157" t="s">
         <v>863</v>
       </c>
-      <c r="C36" s="157" t="s">
+      <c r="D36" s="155" t="s">
         <v>864</v>
-      </c>
-      <c r="D36" s="155" t="s">
-        <v>865</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="14.25">
@@ -25454,13 +25511,13 @@
         <v>4</v>
       </c>
       <c r="B37" s="156" t="s">
+        <v>865</v>
+      </c>
+      <c r="C37" s="157" t="s">
         <v>866</v>
       </c>
-      <c r="C37" s="157" t="s">
+      <c r="D37" s="153" t="s">
         <v>867</v>
-      </c>
-      <c r="D37" s="153" t="s">
-        <v>868</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="14.25">
@@ -25469,10 +25526,10 @@
         <v>364</v>
       </c>
       <c r="C38" s="157" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="D38" s="155" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="14.25">
@@ -25480,13 +25537,13 @@
         <v>4</v>
       </c>
       <c r="B39" s="156" t="s">
+        <v>869</v>
+      </c>
+      <c r="C39" s="157" t="s">
         <v>870</v>
       </c>
-      <c r="C39" s="157" t="s">
+      <c r="D39" s="155" t="s">
         <v>871</v>
-      </c>
-      <c r="D39" s="155" t="s">
-        <v>872</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="14.25">
@@ -25494,7 +25551,7 @@
       <c r="B40" s="140"/>
       <c r="C40" s="140"/>
       <c r="D40" s="154" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="14.25">
@@ -25502,13 +25559,13 @@
         <v>4</v>
       </c>
       <c r="B41" s="156" t="s">
+        <v>873</v>
+      </c>
+      <c r="C41" s="157" t="s">
         <v>874</v>
       </c>
-      <c r="C41" s="157" t="s">
+      <c r="D41" s="155" t="s">
         <v>875</v>
-      </c>
-      <c r="D41" s="155" t="s">
-        <v>876</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="14.25">
@@ -25516,13 +25573,13 @@
         <v>4</v>
       </c>
       <c r="B42" s="156" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="C42" s="157" t="s">
         <v>677</v>
       </c>
       <c r="D42" s="155" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="14.25">
@@ -25530,13 +25587,13 @@
         <v>4</v>
       </c>
       <c r="B43" s="156" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="C43" s="157" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="D43" s="155" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="44" spans="1:4" s="140" customFormat="1" ht="14.25">
@@ -25544,13 +25601,13 @@
         <v>4</v>
       </c>
       <c r="B44" s="156" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="C44" s="157" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="D44" s="155" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="14.25">
@@ -25558,13 +25615,13 @@
         <v>4</v>
       </c>
       <c r="B45" s="156" t="s">
+        <v>881</v>
+      </c>
+      <c r="C45" s="184" t="s">
+        <v>964</v>
+      </c>
+      <c r="D45" s="155" t="s">
         <v>882</v>
-      </c>
-      <c r="C45" s="184" t="s">
-        <v>965</v>
-      </c>
-      <c r="D45" s="155" t="s">
-        <v>883</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="14.25">
@@ -25572,13 +25629,13 @@
         <v>4</v>
       </c>
       <c r="B46" s="156" t="s">
+        <v>883</v>
+      </c>
+      <c r="C46" s="157" t="s">
         <v>884</v>
       </c>
-      <c r="C46" s="157" t="s">
+      <c r="D46" s="155" t="s">
         <v>885</v>
-      </c>
-      <c r="D46" s="155" t="s">
-        <v>886</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="14.25">
@@ -25586,13 +25643,13 @@
         <v>4</v>
       </c>
       <c r="B47" s="156" t="s">
+        <v>886</v>
+      </c>
+      <c r="C47" s="157" t="s">
         <v>887</v>
       </c>
-      <c r="C47" s="157" t="s">
+      <c r="D47" s="155" t="s">
         <v>888</v>
-      </c>
-      <c r="D47" s="155" t="s">
-        <v>889</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="14.25">
@@ -25600,13 +25657,13 @@
         <v>4</v>
       </c>
       <c r="B48" s="156" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="C48" s="157">
         <v>13100000000</v>
       </c>
       <c r="D48" s="155" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="14.25">
@@ -25614,13 +25671,13 @@
         <v>4</v>
       </c>
       <c r="B49" s="156" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="C49" s="157">
         <v>13100001111</v>
       </c>
       <c r="D49" s="155" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="14.25">
@@ -25628,13 +25685,13 @@
         <v>4</v>
       </c>
       <c r="B50" s="156" t="s">
+        <v>893</v>
+      </c>
+      <c r="C50" s="157" t="s">
         <v>894</v>
       </c>
-      <c r="C50" s="157" t="s">
+      <c r="D50" s="155" t="s">
         <v>895</v>
-      </c>
-      <c r="D50" s="155" t="s">
-        <v>896</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="14.25">
@@ -25642,7 +25699,7 @@
       <c r="B51" s="140"/>
       <c r="C51" s="140"/>
       <c r="D51" s="154" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="14.25">
@@ -25650,13 +25707,13 @@
         <v>4</v>
       </c>
       <c r="B52" s="156" t="s">
+        <v>897</v>
+      </c>
+      <c r="C52" s="157" t="s">
         <v>898</v>
       </c>
-      <c r="C52" s="157" t="s">
+      <c r="D52" s="155" t="s">
         <v>899</v>
-      </c>
-      <c r="D52" s="155" t="s">
-        <v>900</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="14.25">
@@ -25664,13 +25721,13 @@
         <v>4</v>
       </c>
       <c r="B53" s="156" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="C53" s="157">
         <v>13211111111</v>
       </c>
       <c r="D53" s="155" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="14.25">
@@ -25678,13 +25735,13 @@
         <v>4</v>
       </c>
       <c r="B54" s="156" t="s">
+        <v>902</v>
+      </c>
+      <c r="C54" s="157" t="s">
+        <v>933</v>
+      </c>
+      <c r="D54" s="155" t="s">
         <v>903</v>
-      </c>
-      <c r="C54" s="157" t="s">
-        <v>934</v>
-      </c>
-      <c r="D54" s="155" t="s">
-        <v>904</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="14.25">
@@ -25692,7 +25749,7 @@
       <c r="B55" s="140"/>
       <c r="C55" s="140"/>
       <c r="D55" s="154" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="14.25">
@@ -25700,13 +25757,13 @@
         <v>4</v>
       </c>
       <c r="B56" s="156" t="s">
+        <v>905</v>
+      </c>
+      <c r="C56" s="157" t="s">
         <v>906</v>
       </c>
-      <c r="C56" s="157" t="s">
-        <v>907</v>
-      </c>
       <c r="D56" s="155" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="14.25">
@@ -25714,13 +25771,13 @@
         <v>4</v>
       </c>
       <c r="B57" s="156" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="C57" s="157">
         <v>13211112222</v>
       </c>
       <c r="D57" s="155" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="14.25">
@@ -25728,13 +25785,13 @@
         <v>4</v>
       </c>
       <c r="B58" s="156" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="C58" s="157" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="D58" s="155" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="14.25">
@@ -25742,7 +25799,7 @@
       <c r="B59" s="140"/>
       <c r="C59" s="140"/>
       <c r="D59" s="154" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="14.25">
@@ -25750,13 +25807,13 @@
         <v>4</v>
       </c>
       <c r="B60" s="156" t="s">
+        <v>910</v>
+      </c>
+      <c r="C60" s="157" t="s">
         <v>911</v>
       </c>
-      <c r="C60" s="157" t="s">
+      <c r="D60" s="155" t="s">
         <v>912</v>
-      </c>
-      <c r="D60" s="155" t="s">
-        <v>913</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="14.25">
@@ -25764,13 +25821,13 @@
         <v>4</v>
       </c>
       <c r="B61" s="156" t="s">
+        <v>913</v>
+      </c>
+      <c r="C61" s="157" t="s">
+        <v>936</v>
+      </c>
+      <c r="D61" s="155" t="s">
         <v>914</v>
-      </c>
-      <c r="C61" s="157" t="s">
-        <v>937</v>
-      </c>
-      <c r="D61" s="155" t="s">
-        <v>915</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="14.25">
@@ -25778,7 +25835,7 @@
         <v>18</v>
       </c>
       <c r="B63" s="138" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="H63" s="140" t="s">
         <v>518</v>
@@ -25789,7 +25846,7 @@
         <v>517</v>
       </c>
       <c r="B64" s="151" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
   </sheetData>
@@ -28555,25 +28612,25 @@
         <v>228</v>
       </c>
       <c r="H22" s="159" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="I22" s="159" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="J22" s="185" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="K22" s="159" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="L22" s="159" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="M22" s="159" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="N22" s="159" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="O22" s="159" t="s">
         <v>684</v>
@@ -28585,7 +28642,7 @@
         <v>229</v>
       </c>
       <c r="R22" s="159" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="S22" s="160" t="s">
         <v>170</v>
@@ -28612,22 +28669,22 @@
         <v>170</v>
       </c>
       <c r="AA22" s="159" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="AB22" s="185" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="AC22" s="159" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="AD22" s="159" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="AE22" s="159" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="AF22" s="159" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="AG22" s="160" t="s">
         <v>170</v>
@@ -28651,31 +28708,31 @@
         <v>170</v>
       </c>
       <c r="AN22" s="159" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="AO22" s="159" t="s">
         <v>228</v>
       </c>
       <c r="AP22" s="159" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="AQ22" s="159" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="AR22" s="185" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="AS22" s="159" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="AT22" s="159" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="AU22" s="159" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="AV22" s="159" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="AW22" s="160" t="s">
         <v>170</v>
@@ -28726,31 +28783,31 @@
         <v>170</v>
       </c>
       <c r="BM22" s="159" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="BN22" s="159" t="s">
+        <v>945</v>
+      </c>
+      <c r="BO22" s="160" t="s">
+        <v>170</v>
+      </c>
+      <c r="BP22" s="160" t="s">
+        <v>170</v>
+      </c>
+      <c r="BQ22" s="160" t="s">
+        <v>170</v>
+      </c>
+      <c r="BR22" s="160" t="s">
+        <v>170</v>
+      </c>
+      <c r="BS22" s="160" t="s">
+        <v>170</v>
+      </c>
+      <c r="BT22" s="159" t="s">
         <v>946</v>
       </c>
-      <c r="BO22" s="160" t="s">
-        <v>170</v>
-      </c>
-      <c r="BP22" s="160" t="s">
-        <v>170</v>
-      </c>
-      <c r="BQ22" s="160" t="s">
-        <v>170</v>
-      </c>
-      <c r="BR22" s="160" t="s">
-        <v>170</v>
-      </c>
-      <c r="BS22" s="160" t="s">
-        <v>170</v>
-      </c>
-      <c r="BT22" s="159" t="s">
-        <v>947</v>
-      </c>
       <c r="BU22" s="159" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="BV22" s="160" t="s">
         <v>170</v>
@@ -28759,7 +28816,7 @@
         <v>170</v>
       </c>
       <c r="BX22" s="159" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="BY22" s="160" t="s">
         <v>170</v>
@@ -28771,19 +28828,19 @@
         <v>170</v>
       </c>
       <c r="CB22" s="159" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="CC22" s="159" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="CD22" s="159" t="s">
         <v>615</v>
       </c>
       <c r="CE22" s="159" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="CF22" s="159" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="CG22" s="160" t="s">
         <v>170</v>
@@ -28792,16 +28849,16 @@
         <v>170</v>
       </c>
       <c r="CI22" s="159" t="s">
+        <v>948</v>
+      </c>
+      <c r="CJ22" s="159" t="s">
         <v>949</v>
       </c>
-      <c r="CJ22" s="159" t="s">
+      <c r="CK22" s="159" t="s">
         <v>950</v>
       </c>
-      <c r="CK22" s="159" t="s">
-        <v>951</v>
-      </c>
       <c r="CL22" s="159" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="CM22" s="160" t="s">
         <v>170</v>
@@ -28819,22 +28876,22 @@
         <v>220</v>
       </c>
       <c r="CR22" s="159" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="CS22" s="160" t="s">
         <v>170</v>
       </c>
       <c r="CT22" s="159" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="CU22" s="159" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="CV22" s="160" t="s">
         <v>170</v>
       </c>
       <c r="CW22" s="159" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="CX22" s="160" t="s">
         <v>170</v>
@@ -28882,13 +28939,13 @@
         <v>170</v>
       </c>
       <c r="DM22" s="159" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="DN22" s="159" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="DO22" s="159" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="DP22" s="160" t="s">
         <v>170</v>
@@ -30696,17 +30753,17 @@
         <v>250</v>
       </c>
       <c r="B34" s="175" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="35" spans="1:142" s="171" customFormat="1">
       <c r="B35" s="179" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="36" spans="1:142" s="171" customFormat="1">
       <c r="B36" s="178" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="C36" s="177" t="s">
         <v>19</v>
@@ -30721,10 +30778,10 @@
         <v>21</v>
       </c>
       <c r="G36" s="177" t="s">
+        <v>994</v>
+      </c>
+      <c r="H36" s="177" t="s">
         <v>995</v>
-      </c>
-      <c r="H36" s="177" t="s">
-        <v>996</v>
       </c>
       <c r="I36" s="177" t="s">
         <v>43</v>
@@ -30733,28 +30790,28 @@
         <v>37</v>
       </c>
       <c r="K36" s="177" t="s">
+        <v>996</v>
+      </c>
+      <c r="L36" s="177" t="s">
         <v>997</v>
       </c>
-      <c r="L36" s="177" t="s">
+      <c r="M36" s="177" t="s">
         <v>998</v>
       </c>
-      <c r="M36" s="177" t="s">
+      <c r="N36" s="177" t="s">
         <v>999</v>
       </c>
-      <c r="N36" s="177" t="s">
+      <c r="O36" s="177" t="s">
         <v>1000</v>
       </c>
-      <c r="O36" s="177" t="s">
+      <c r="P36" s="177" t="s">
         <v>1001</v>
       </c>
-      <c r="P36" s="177" t="s">
+      <c r="Q36" s="177" t="s">
         <v>1002</v>
       </c>
-      <c r="Q36" s="177" t="s">
+      <c r="R36" s="177" t="s">
         <v>1003</v>
-      </c>
-      <c r="R36" s="177" t="s">
-        <v>1004</v>
       </c>
       <c r="S36" s="177" t="s">
         <v>440</v>
@@ -30772,25 +30829,25 @@
         <v>36</v>
       </c>
       <c r="X36" s="177" t="s">
+        <v>1004</v>
+      </c>
+      <c r="Y36" s="177" t="s">
         <v>1005</v>
       </c>
-      <c r="Y36" s="177" t="s">
+      <c r="Z36" s="177" t="s">
         <v>1006</v>
       </c>
-      <c r="Z36" s="177" t="s">
+      <c r="AA36" s="177" t="s">
         <v>1007</v>
       </c>
-      <c r="AA36" s="177" t="s">
+      <c r="AB36" s="177" t="s">
         <v>1008</v>
       </c>
-      <c r="AB36" s="177" t="s">
+      <c r="AC36" s="177" t="s">
         <v>1009</v>
       </c>
-      <c r="AC36" s="177" t="s">
+      <c r="AD36" s="177" t="s">
         <v>1010</v>
-      </c>
-      <c r="AD36" s="177" t="s">
-        <v>1011</v>
       </c>
     </row>
     <row r="37" spans="1:142">
@@ -30811,7 +30868,7 @@
         <v>170</v>
       </c>
       <c r="G37" s="190" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="H37" s="190" t="s">
         <v>220</v>
@@ -30826,7 +30883,7 @@
         <v>581</v>
       </c>
       <c r="L37" s="190" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="M37" s="191" t="s">
         <v>170</v>
@@ -31020,7 +31077,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="171" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="171" customFormat="1" ht="14.25">
@@ -31034,10 +31091,10 @@
         <v>18</v>
       </c>
       <c r="B4" s="171" t="s">
+        <v>794</v>
+      </c>
+      <c r="I4" s="171" t="s">
         <v>795</v>
-      </c>
-      <c r="I4" s="171" t="s">
-        <v>796</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="64" customFormat="1" ht="14.25">
@@ -31109,7 +31166,7 @@
         <v>517</v>
       </c>
       <c r="B11" s="166" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="C11" s="170"/>
       <c r="D11" s="167"/>
@@ -31119,7 +31176,7 @@
         <v>517</v>
       </c>
       <c r="B12" s="171" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="64" customFormat="1" ht="14.25">
@@ -33893,25 +33950,25 @@
         <v>228</v>
       </c>
       <c r="H22" s="185" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="I22" s="185" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="J22" s="185" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="K22" s="185" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="L22" s="185" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="M22" s="185" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="N22" s="185" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="O22" s="185" t="s">
         <v>684</v>
@@ -33923,7 +33980,7 @@
         <v>229</v>
       </c>
       <c r="R22" s="185" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="S22" s="186" t="s">
         <v>170</v>
@@ -33950,22 +34007,22 @@
         <v>170</v>
       </c>
       <c r="AA22" s="185" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="AB22" s="185" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="AC22" s="185" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="AD22" s="185" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="AE22" s="185" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="AF22" s="185" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="AG22" s="186" t="s">
         <v>170</v>
@@ -33989,31 +34046,31 @@
         <v>170</v>
       </c>
       <c r="AN22" s="185" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="AO22" s="185" t="s">
         <v>228</v>
       </c>
       <c r="AP22" s="185" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="AQ22" s="185" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="AR22" s="185" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="AS22" s="185" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="AT22" s="185" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="AU22" s="185" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="AV22" s="185" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="AW22" s="186" t="s">
         <v>170</v>
@@ -34064,31 +34121,31 @@
         <v>170</v>
       </c>
       <c r="BM22" s="185" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="BN22" s="185" t="s">
+        <v>945</v>
+      </c>
+      <c r="BO22" s="186" t="s">
+        <v>170</v>
+      </c>
+      <c r="BP22" s="186" t="s">
+        <v>170</v>
+      </c>
+      <c r="BQ22" s="186" t="s">
+        <v>170</v>
+      </c>
+      <c r="BR22" s="186" t="s">
+        <v>170</v>
+      </c>
+      <c r="BS22" s="186" t="s">
+        <v>170</v>
+      </c>
+      <c r="BT22" s="185" t="s">
         <v>946</v>
       </c>
-      <c r="BO22" s="186" t="s">
-        <v>170</v>
-      </c>
-      <c r="BP22" s="186" t="s">
-        <v>170</v>
-      </c>
-      <c r="BQ22" s="186" t="s">
-        <v>170</v>
-      </c>
-      <c r="BR22" s="186" t="s">
-        <v>170</v>
-      </c>
-      <c r="BS22" s="186" t="s">
-        <v>170</v>
-      </c>
-      <c r="BT22" s="185" t="s">
-        <v>947</v>
-      </c>
       <c r="BU22" s="185" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="BV22" s="186" t="s">
         <v>170</v>
@@ -34097,7 +34154,7 @@
         <v>170</v>
       </c>
       <c r="BX22" s="185" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="BY22" s="186" t="s">
         <v>170</v>
@@ -34109,19 +34166,19 @@
         <v>170</v>
       </c>
       <c r="CB22" s="185" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="CC22" s="185" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="CD22" s="185" t="s">
         <v>615</v>
       </c>
       <c r="CE22" s="185" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="CF22" s="185" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="CG22" s="186" t="s">
         <v>170</v>
@@ -34130,16 +34187,16 @@
         <v>170</v>
       </c>
       <c r="CI22" s="185" t="s">
+        <v>948</v>
+      </c>
+      <c r="CJ22" s="185" t="s">
         <v>949</v>
       </c>
-      <c r="CJ22" s="185" t="s">
+      <c r="CK22" s="185" t="s">
         <v>950</v>
       </c>
-      <c r="CK22" s="185" t="s">
-        <v>951</v>
-      </c>
       <c r="CL22" s="185" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="CM22" s="186" t="s">
         <v>170</v>
@@ -34157,22 +34214,22 @@
         <v>220</v>
       </c>
       <c r="CR22" s="185" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="CS22" s="186" t="s">
         <v>170</v>
       </c>
       <c r="CT22" s="185" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="CU22" s="185" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="CV22" s="186" t="s">
         <v>170</v>
       </c>
       <c r="CW22" s="185" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="CX22" s="186" t="s">
         <v>170</v>
@@ -34220,13 +34277,13 @@
         <v>170</v>
       </c>
       <c r="DM22" s="185" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="DN22" s="185" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="DO22" s="185" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="DP22" s="186" t="s">
         <v>170</v>
@@ -36034,18 +36091,18 @@
         <v>250</v>
       </c>
       <c r="B34" s="175" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="35" spans="1:142" s="129" customFormat="1">
       <c r="A35" s="171"/>
       <c r="B35" s="179" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="36" spans="1:142" s="129" customFormat="1">
       <c r="B36" s="178" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="C36" s="177" t="s">
         <v>19</v>
@@ -36060,10 +36117,10 @@
         <v>21</v>
       </c>
       <c r="G36" s="177" t="s">
+        <v>994</v>
+      </c>
+      <c r="H36" s="177" t="s">
         <v>995</v>
-      </c>
-      <c r="H36" s="177" t="s">
-        <v>996</v>
       </c>
       <c r="I36" s="177" t="s">
         <v>43</v>
@@ -36072,28 +36129,28 @@
         <v>37</v>
       </c>
       <c r="K36" s="177" t="s">
+        <v>996</v>
+      </c>
+      <c r="L36" s="177" t="s">
         <v>997</v>
       </c>
-      <c r="L36" s="177" t="s">
+      <c r="M36" s="177" t="s">
         <v>998</v>
       </c>
-      <c r="M36" s="177" t="s">
+      <c r="N36" s="177" t="s">
         <v>999</v>
       </c>
-      <c r="N36" s="177" t="s">
+      <c r="O36" s="177" t="s">
         <v>1000</v>
       </c>
-      <c r="O36" s="177" t="s">
+      <c r="P36" s="177" t="s">
         <v>1001</v>
       </c>
-      <c r="P36" s="177" t="s">
+      <c r="Q36" s="177" t="s">
         <v>1002</v>
       </c>
-      <c r="Q36" s="177" t="s">
+      <c r="R36" s="177" t="s">
         <v>1003</v>
-      </c>
-      <c r="R36" s="177" t="s">
-        <v>1004</v>
       </c>
       <c r="S36" s="177" t="s">
         <v>440</v>
@@ -36111,25 +36168,25 @@
         <v>36</v>
       </c>
       <c r="X36" s="177" t="s">
+        <v>1004</v>
+      </c>
+      <c r="Y36" s="177" t="s">
         <v>1005</v>
       </c>
-      <c r="Y36" s="177" t="s">
+      <c r="Z36" s="177" t="s">
         <v>1006</v>
       </c>
-      <c r="Z36" s="177" t="s">
+      <c r="AA36" s="177" t="s">
         <v>1007</v>
       </c>
-      <c r="AA36" s="177" t="s">
+      <c r="AB36" s="177" t="s">
         <v>1008</v>
       </c>
-      <c r="AB36" s="177" t="s">
+      <c r="AC36" s="177" t="s">
         <v>1009</v>
       </c>
-      <c r="AC36" s="177" t="s">
+      <c r="AD36" s="177" t="s">
         <v>1010</v>
-      </c>
-      <c r="AD36" s="177" t="s">
-        <v>1011</v>
       </c>
     </row>
     <row r="37" spans="1:142" s="188" customFormat="1">
@@ -36150,7 +36207,7 @@
         <v>170</v>
       </c>
       <c r="G37" s="190" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="H37" s="190" t="s">
         <v>220</v>
@@ -36165,7 +36222,7 @@
         <v>581</v>
       </c>
       <c r="L37" s="190" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="M37" s="191" t="s">
         <v>170</v>
@@ -36180,7 +36237,7 @@
         <v>170</v>
       </c>
       <c r="Q37" s="202" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="R37" s="190" t="s">
         <v>229</v>
@@ -36201,7 +36258,7 @@
         <v>229</v>
       </c>
       <c r="X37" s="194" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="Y37" s="194" t="s">
         <v>761</v>
@@ -36364,7 +36421,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="171" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="171" customFormat="1" ht="14.25">
@@ -36378,10 +36435,10 @@
         <v>18</v>
       </c>
       <c r="B4" s="171" t="s">
+        <v>794</v>
+      </c>
+      <c r="I4" s="171" t="s">
         <v>795</v>
-      </c>
-      <c r="I4" s="171" t="s">
-        <v>796</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="113" customFormat="1" ht="14.25">
@@ -36406,7 +36463,7 @@
       <c r="C6" s="70"/>
       <c r="F6" s="70"/>
       <c r="J6" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="113" customFormat="1" ht="15">
@@ -36419,7 +36476,7 @@
       <c r="C7" s="70"/>
       <c r="F7" s="70"/>
       <c r="J7" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="113" customFormat="1" ht="14.25">
@@ -36435,7 +36492,7 @@
         <v>517</v>
       </c>
       <c r="B9" s="171" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="113" customFormat="1" ht="14.25">
@@ -36459,7 +36516,7 @@
         <v>517</v>
       </c>
       <c r="B12" s="171" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="113" customFormat="1" ht="14.25">
@@ -36539,7 +36596,7 @@
         <v>517</v>
       </c>
       <c r="B23" s="171" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="C23" s="173"/>
     </row>
@@ -36552,7 +36609,7 @@
       </c>
       <c r="C24" s="173"/>
       <c r="H24" s="171" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="171" customFormat="1" ht="14.25">
@@ -36560,7 +36617,7 @@
         <v>517</v>
       </c>
       <c r="B25" s="171" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="C25" s="173"/>
     </row>
@@ -36616,7 +36673,7 @@
       </c>
       <c r="C31" s="173"/>
       <c r="D31" s="171" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="32" spans="1:10" s="171" customFormat="1" ht="14.25">
@@ -36628,7 +36685,7 @@
       </c>
       <c r="C32" s="173"/>
       <c r="D32" s="171" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="33" spans="1:8" s="171" customFormat="1" ht="14.25">
@@ -36880,7 +36937,7 @@
         <v>735</v>
       </c>
       <c r="J4" s="185" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="K4" s="186" t="s">
         <v>170</v>
@@ -39446,25 +39503,25 @@
         <v>228</v>
       </c>
       <c r="H22" s="185" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="I22" s="185" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="J22" s="185" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="K22" s="185" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="L22" s="185" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="M22" s="185" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="N22" s="185" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="O22" s="185" t="s">
         <v>684</v>
@@ -39476,7 +39533,7 @@
         <v>229</v>
       </c>
       <c r="R22" s="185" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="S22" s="186" t="s">
         <v>170</v>
@@ -39503,22 +39560,22 @@
         <v>170</v>
       </c>
       <c r="AA22" s="185" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="AB22" s="185" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="AC22" s="185" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="AD22" s="185" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="AE22" s="185" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="AF22" s="185" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="AG22" s="186" t="s">
         <v>170</v>
@@ -39542,31 +39599,31 @@
         <v>170</v>
       </c>
       <c r="AN22" s="185" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="AO22" s="185" t="s">
         <v>228</v>
       </c>
       <c r="AP22" s="185" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="AQ22" s="185" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="AR22" s="185" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="AS22" s="185" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="AT22" s="185" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="AU22" s="185" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="AV22" s="185" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="AW22" s="186" t="s">
         <v>170</v>
@@ -39617,31 +39674,31 @@
         <v>170</v>
       </c>
       <c r="BM22" s="185" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="BN22" s="185" t="s">
+        <v>945</v>
+      </c>
+      <c r="BO22" s="186" t="s">
+        <v>170</v>
+      </c>
+      <c r="BP22" s="186" t="s">
+        <v>170</v>
+      </c>
+      <c r="BQ22" s="186" t="s">
+        <v>170</v>
+      </c>
+      <c r="BR22" s="186" t="s">
+        <v>170</v>
+      </c>
+      <c r="BS22" s="186" t="s">
+        <v>170</v>
+      </c>
+      <c r="BT22" s="185" t="s">
         <v>946</v>
       </c>
-      <c r="BO22" s="186" t="s">
-        <v>170</v>
-      </c>
-      <c r="BP22" s="186" t="s">
-        <v>170</v>
-      </c>
-      <c r="BQ22" s="186" t="s">
-        <v>170</v>
-      </c>
-      <c r="BR22" s="186" t="s">
-        <v>170</v>
-      </c>
-      <c r="BS22" s="186" t="s">
-        <v>170</v>
-      </c>
-      <c r="BT22" s="185" t="s">
-        <v>947</v>
-      </c>
       <c r="BU22" s="185" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="BV22" s="186" t="s">
         <v>170</v>
@@ -39650,7 +39707,7 @@
         <v>170</v>
       </c>
       <c r="BX22" s="185" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="BY22" s="186" t="s">
         <v>170</v>
@@ -39662,19 +39719,19 @@
         <v>170</v>
       </c>
       <c r="CB22" s="185" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="CC22" s="185" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="CD22" s="185" t="s">
         <v>615</v>
       </c>
       <c r="CE22" s="185" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="CF22" s="185" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="CG22" s="186" t="s">
         <v>170</v>
@@ -39683,16 +39740,16 @@
         <v>170</v>
       </c>
       <c r="CI22" s="185" t="s">
+        <v>948</v>
+      </c>
+      <c r="CJ22" s="185" t="s">
         <v>949</v>
       </c>
-      <c r="CJ22" s="185" t="s">
+      <c r="CK22" s="185" t="s">
         <v>950</v>
       </c>
-      <c r="CK22" s="185" t="s">
-        <v>951</v>
-      </c>
       <c r="CL22" s="185" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="CM22" s="186" t="s">
         <v>170</v>
@@ -39710,22 +39767,22 @@
         <v>220</v>
       </c>
       <c r="CR22" s="185" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="CS22" s="186" t="s">
         <v>170</v>
       </c>
       <c r="CT22" s="185" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="CU22" s="185" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="CV22" s="186" t="s">
         <v>170</v>
       </c>
       <c r="CW22" s="185" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="CX22" s="186" t="s">
         <v>170</v>
@@ -39773,13 +39830,13 @@
         <v>170</v>
       </c>
       <c r="DM22" s="185" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="DN22" s="185" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="DO22" s="185" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="DP22" s="186" t="s">
         <v>170</v>
@@ -41587,17 +41644,17 @@
         <v>250</v>
       </c>
       <c r="B34" s="175" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="35" spans="1:142">
       <c r="B35" s="179" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="36" spans="1:142">
       <c r="B36" s="178" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="C36" s="177" t="s">
         <v>19</v>
@@ -41612,10 +41669,10 @@
         <v>21</v>
       </c>
       <c r="G36" s="177" t="s">
+        <v>994</v>
+      </c>
+      <c r="H36" s="177" t="s">
         <v>995</v>
-      </c>
-      <c r="H36" s="177" t="s">
-        <v>996</v>
       </c>
       <c r="I36" s="177" t="s">
         <v>43</v>
@@ -41624,28 +41681,28 @@
         <v>37</v>
       </c>
       <c r="K36" s="177" t="s">
+        <v>996</v>
+      </c>
+      <c r="L36" s="177" t="s">
         <v>997</v>
       </c>
-      <c r="L36" s="177" t="s">
+      <c r="M36" s="177" t="s">
         <v>998</v>
       </c>
-      <c r="M36" s="177" t="s">
+      <c r="N36" s="177" t="s">
         <v>999</v>
       </c>
-      <c r="N36" s="177" t="s">
+      <c r="O36" s="177" t="s">
         <v>1000</v>
       </c>
-      <c r="O36" s="177" t="s">
+      <c r="P36" s="177" t="s">
         <v>1001</v>
       </c>
-      <c r="P36" s="177" t="s">
+      <c r="Q36" s="177" t="s">
         <v>1002</v>
       </c>
-      <c r="Q36" s="177" t="s">
+      <c r="R36" s="177" t="s">
         <v>1003</v>
-      </c>
-      <c r="R36" s="177" t="s">
-        <v>1004</v>
       </c>
       <c r="S36" s="177" t="s">
         <v>440</v>
@@ -41663,25 +41720,25 @@
         <v>36</v>
       </c>
       <c r="X36" s="177" t="s">
+        <v>1004</v>
+      </c>
+      <c r="Y36" s="177" t="s">
         <v>1005</v>
       </c>
-      <c r="Y36" s="177" t="s">
+      <c r="Z36" s="177" t="s">
         <v>1006</v>
       </c>
-      <c r="Z36" s="177" t="s">
+      <c r="AA36" s="177" t="s">
         <v>1007</v>
       </c>
-      <c r="AA36" s="177" t="s">
+      <c r="AB36" s="177" t="s">
         <v>1008</v>
       </c>
-      <c r="AB36" s="177" t="s">
+      <c r="AC36" s="177" t="s">
         <v>1009</v>
       </c>
-      <c r="AC36" s="177" t="s">
+      <c r="AD36" s="177" t="s">
         <v>1010</v>
-      </c>
-      <c r="AD36" s="177" t="s">
-        <v>1011</v>
       </c>
     </row>
     <row r="37" spans="1:142" s="192" customFormat="1">
@@ -41702,7 +41759,7 @@
         <v>170</v>
       </c>
       <c r="G37" s="194" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="H37" s="194" t="s">
         <v>220</v>
@@ -41717,7 +41774,7 @@
         <v>581</v>
       </c>
       <c r="L37" s="194" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="M37" s="195" t="s">
         <v>170</v>
@@ -41732,7 +41789,7 @@
         <v>170</v>
       </c>
       <c r="Q37" s="202" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="R37" s="194" t="s">
         <v>229</v>
@@ -41753,7 +41810,7 @@
         <v>229</v>
       </c>
       <c r="X37" s="194" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="Y37" s="194" t="s">
         <v>761</v>
@@ -41762,7 +41819,7 @@
         <v>732</v>
       </c>
       <c r="AA37" s="196" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="AB37" s="185" t="s">
         <v>554</v>

</xml_diff>